<commit_message>
complete upload and import data sample app
</commit_message>
<xml_diff>
--- a/uploads/users.xlsx
+++ b/uploads/users.xlsx
@@ -5,43 +5,63 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="198" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>mobile</t>
+    <t>mobile number</t>
   </si>
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>joseph</t>
-  </si>
-  <si>
-    <t>j@gmail.com</t>
+    <t>joseph chingalo</t>
+  </si>
+  <si>
+    <t>profschingalo@gmail.com</t>
+  </si>
+  <si>
+    <t>philibert chingalo</t>
+  </si>
+  <si>
+    <t>pchingalo@gmail.com</t>
+  </si>
+  <si>
+    <t>eric chingalo</t>
+  </si>
+  <si>
+    <t>echingalo@gmail.com</t>
+  </si>
+  <si>
+    <t>ester chingalo</t>
+  </si>
+  <si>
+    <t>esterchingalo@gmail.com</t>
+  </si>
+  <si>
+    <t>raphael chingalo</t>
+  </si>
+  <si>
+    <t>rchingalo@yahoo.com</t>
   </si>
   <si>
     <t>chingalo</t>
   </si>
   <si>
-    <t>chingalo@yahoo.com</t>
-  </si>
-  <si>
-    <t>raphael</t>
-  </si>
-  <si>
-    <t>rchingalo@yahoo.com</t>
+    <t>chingalo@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -53,9 +73,11 @@
   </numFmts>
   <fonts count="5">
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -73,10 +95,12 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
+      <u val="single"/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -96,7 +120,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -120,24 +144,29 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="4" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="20">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
     <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
     <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -147,20 +176,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D7" activeCellId="0" pane="topLeft" sqref="D7"/>
+      <selection activeCell="A15" activeCellId="0" pane="topLeft" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.4291497975708"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.1417004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="20.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.5748987854251"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -171,51 +202,160 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>787231123</v>
+        <v>687167637</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>783123412</v>
+        <v>784331423</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>687232322</v>
+        <v>734523654</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>784331428</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
+      <c r="A6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>782676666</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
+      <c r="A7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>718922311</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
+      <c r="A8" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
+      <c r="A9" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>784331423</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="j@gmail.com" ref="C2" r:id="rId1"/>
-    <hyperlink display="chingalo@yahoo.com" ref="C3" r:id="rId2"/>
-    <hyperlink display="rchingalo@yahoo.com" ref="C4" r:id="rId3"/>
+    <hyperlink display="profschingalo@gmail.com" ref="C2" r:id="rId1"/>
+    <hyperlink display="pchingalo@gmail.com" ref="C3" r:id="rId2"/>
+    <hyperlink display="echingalo@gmail.com" ref="C4" r:id="rId3"/>
+    <hyperlink display="esterchingalo@gmail.com" ref="C5" r:id="rId4"/>
+    <hyperlink display="rchingalo@yahoo.com" ref="C6" r:id="rId5"/>
+    <hyperlink display="chingalo@gmail.com" ref="C7" r:id="rId6"/>
+    <hyperlink display="profschingalo@gmail.com" ref="C8" r:id="rId7"/>
+    <hyperlink display="pchingalo@gmail.com" ref="C9" r:id="rId8"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>